<commit_message>
Added Selenium code and test document
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="448" documentId="11_F25DC773A252ABDACC1048CBA19B48FE5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65094348-B83C-4598-A85B-E9312254807C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="12" activeTab="15" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logo Verification" sheetId="1" r:id="rId1"/>
@@ -4383,8 +4383,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8765,8 +8765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{084D5CB2-7DCF-4C06-9D52-7EA274E0D594}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G21"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11325,7 +11325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{608A4F99-9251-46A2-B8EA-17689A360606}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated test cases and added new test files
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b45239f61cd31ee/Documents/Project/Flipkart Clone Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="448" documentId="11_F25DC773A252ABDACC1048CBA19B48FE5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65094348-B83C-4598-A85B-E9312254807C}"/>
+  <xr:revisionPtr revIDLastSave="471" documentId="11_F25DC773A252ABDACC1048CBA19B48FE5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D18AB722-DDEE-4E00-8C40-571793743C27}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="2508" yWindow="2508" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logo Verification" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2293" uniqueCount="1285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="1292">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -3920,6 +3920,29 @@
   </si>
   <si>
     <t>All elements are accessible using keyboard navigation.</t>
+  </si>
+  <si>
+    <t>Logo Clearly Visible</t>
+  </si>
+  <si>
+    <t>P0</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Mail-HarryVerma@hotmail.com
+Password-Harry@45</t>
+  </si>
+  <si>
+    <t>Mail-HarryVerma@hotmail.com
+Password-Harry@46</t>
   </si>
 </sst>
 </file>
@@ -4383,8 +4406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4459,9 +4482,15 @@
       <c r="G2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="H2" s="2" t="s">
+        <v>1285</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -4486,9 +4515,15 @@
       <c r="G3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -4513,9 +4548,15 @@
       <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>1289</v>
+      </c>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -8125,8 +8166,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8952A9-0E18-4AAB-AF8F-289943CDDAB2}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F21"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8195,15 +8236,21 @@
       <c r="E2" s="2" t="s">
         <v>1164</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>15</v>
+      <c r="F2" s="2" t="s">
+        <v>1290</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>1184</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="H2" s="2" t="s">
+        <v>1184</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -8222,15 +8269,21 @@
       <c r="E3" s="2" t="s">
         <v>1165</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>15</v>
+      <c r="F3" s="2" t="s">
+        <v>1291</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>1185</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>1185</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -11965,8 +12018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91468A32-D5D4-418E-A278-7B66A86CD37A}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12112,13 +12165,21 @@
       <c r="E5" s="2" t="s">
         <v>439</v>
       </c>
-      <c r="F5" s="3"/>
+      <c r="F5" s="2" t="s">
+        <v>1290</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>459</v>
       </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="H5" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K5" s="5"/>
     </row>
     <row r="6" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added new test case TC005 and updated LoginPage
</commit_message>
<xml_diff>
--- a/Test Cases.xlsx
+++ b/Test Cases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b45239f61cd31ee/Documents/Project/Flipkart Clone Testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0b45239f61cd31ee/Documents/Project/Flipkart Clone Testing/Flipkart-Clone-Automation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="471" documentId="11_F25DC773A252ABDACC1048CBA19B48FE5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D18AB722-DDEE-4E00-8C40-571793743C27}"/>
+  <xr:revisionPtr revIDLastSave="496" documentId="11_F25DC773A252ABDACC1048CBA19B48FE5BDE58ED" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07828E9D-C586-49E0-A15E-A03741FBA396}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Logo Verification" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2312" uniqueCount="1292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2327" uniqueCount="1293">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -3943,6 +3943,10 @@
   <si>
     <t>Mail-HarryVerma@hotmail.com
 Password-Harry@46</t>
+  </si>
+  <si>
+    <t>Mail-HarryVerma@hotmail.com
+Password-Harry</t>
   </si>
 </sst>
 </file>
@@ -4135,10 +4139,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8166,7 +8166,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A8952A9-0E18-4AAB-AF8F-289943CDDAB2}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J3"/>
     </sheetView>
   </sheetViews>
@@ -9458,7 +9458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE62874-428E-4FF3-AE63-AD313CD43970}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
@@ -10738,7 +10738,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E7C75F1-A169-4D4A-9676-403FCB81DB90}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B21"/>
     </sheetView>
   </sheetViews>
@@ -12018,8 +12018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91468A32-D5D4-418E-A278-7B66A86CD37A}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12094,9 +12094,15 @@
       <c r="G2" s="2" t="s">
         <v>456</v>
       </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="H2" s="2" t="s">
+        <v>456</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K2" s="5"/>
     </row>
     <row r="3" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -12115,13 +12121,21 @@
       <c r="E3" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G3" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K3" s="5"/>
     </row>
     <row r="4" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -12140,13 +12154,21 @@
       <c r="E4" s="2" t="s">
         <v>438</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>15</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>458</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K4" s="5"/>
     </row>
     <row r="5" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
@@ -12198,13 +12220,21 @@
       <c r="E6" s="2" t="s">
         <v>440</v>
       </c>
-      <c r="F6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>1292</v>
+      </c>
       <c r="G6" s="2" t="s">
         <v>460</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="H6" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>1287</v>
+      </c>
       <c r="K6" s="5"/>
     </row>
     <row r="7" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>